<commit_message>
regression all as train and all as valid
</commit_message>
<xml_diff>
--- a/data/data_493.xlsx
+++ b/data/data_493.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2348DD6-37FD-4C85-A0A7-6BC2F52219A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FEA04A-FB06-4955-90AE-008BA3EA7C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14325" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
   <dimension ref="A1:V496"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>